<commit_message>
updated math_vision.py to load appropriate classes for the model
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>model</t>
   </si>
@@ -22,6 +22,9 @@
     <t>description</t>
   </si>
   <si>
+    <t>char_to_num</t>
+  </si>
+  <si>
     <t>math_vision</t>
   </si>
   <si>
@@ -31,6 +34,18 @@
     <t>Designed to distinguish alphabets, special characters and numbers (89 characters) [Note: not reliable]</t>
   </si>
   <si>
+    <t>{
+    '100': 0, '101': 1, '102': 2, '103': 3, '104': 4, '105': 5, '106': 6, '107': 7, '108': 8, '109': 9, '110': 10, '111': 11,
+    '112': 12, '113': 13, '114': 14, '115': 15, '116': 16, '117': 17, '118': 18, '119': 19, '120': 20, '121': 21, '122': 22,
+    '123': 23, '124': 24, '125': 25, '33': 26, '35': 27, '36': 28, '37': 29, '38': 30, '40': 31, '41': 32, '42': 33, '43': 34,
+    '44': 35, '45': 36, '46': 37, '47': 38, '48': 39, '49': 40, '50': 41, '51': 42, '52': 43, '53': 44, '54': 45, '55': 46,
+    '56': 47, '57': 48, '58': 49, '59': 50, '60': 51, '61': 52, '62': 53, '63': 54, '64': 55, '65': 56, '66': 57, '67': 58,
+    '68': 59, '69': 60, '70': 61, '71': 62, '72': 63, '73': 64, '74': 65, '75': 66, '76': 67, '77': 68, '78': 69, '79': 70,
+    '80': 71, '81': 72, '82': 73, '83': 74, '84': 75, '85': 76, '86': 77, '87': 78, '88': 79, '89': 80, '90': 81, '91': 82,
+    '93': 83, '94': 84, '95': 85, '97': 86, '98': 87, '99': 88
+}</t>
+  </si>
+  <si>
     <t>tuned_math_vison</t>
   </si>
   <si>
@@ -38,13 +53,26 @@
   </si>
   <si>
     <t>Tuned version of the math_vision model trained on a fine tuning dataset, blunders less frequently</t>
+  </si>
+  <si>
+    <t>numbers_only_math_vision</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1hdRCBXIYLzbooTxN92mqxI0C0yiEI5hX/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Math vision model designed to only predict numerical figures and special characters (much more reliable)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'101': 0, '120': 1, '123': 2, '124': 3, '125': 4, '33': 5, '35': 6, '36': 7, '37': 8, '38': 9, '40': 10, '41': 11, '42': 12, '43': 13, '44': 14, '45': 15, '46': 16, '47': 17, '48': 18, '49': 19, '50': 20, '51': 21, '52': 22, '53': 23, '54': 24, '55': 25, '56': 26, '57': 27, '58': 28, '59': 29, '60': 30, '61': 31, '62': 32, '63': 33, '64': 34, '88': 35, '91': 36, '93': 37, '94': 38, '95': 39, '97': 40}
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -55,6 +83,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <u/>
@@ -75,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -83,6 +115,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -301,9 +336,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.13"/>
-    <col customWidth="1" min="2" max="2" width="60.38"/>
-    <col customWidth="1" min="3" max="3" width="20.38"/>
+    <col customWidth="1" min="1" max="1" width="22.13"/>
+    <col customWidth="1" min="2" max="2" width="68.5"/>
+    <col customWidth="1" min="3" max="3" width="79.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -316,34 +351,58 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
     <hyperlink r:id="rId2" ref="B3"/>
+    <hyperlink r:id="rId3" ref="B4"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>